<commit_message>
new logging, only one entry box.
</commit_message>
<xml_diff>
--- a/data given to time tracker.xlsx
+++ b/data given to time tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harsh24/Desktop/Time_Tracker_Pro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEAFF21B-F3B2-C544-B169-B73BF40D04B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B516A533-6465-E344-A874-23024F50D4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16920" xr2:uid="{EB65E887-148F-0A42-8DF7-046F7B9F5706}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>column a</t>
-  </si>
-  <si>
-    <t>column b</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>&lt;time_a&gt;&lt;date_a&gt;</t>
   </si>
@@ -57,17 +50,44 @@
     <t>Not Urgent</t>
   </si>
   <si>
-    <t>Important</t>
-  </si>
-  <si>
     <t>Not Important</t>
+  </si>
+  <si>
+    <t>old:</t>
+  </si>
+  <si>
+    <t>new:</t>
+  </si>
+  <si>
+    <t>&lt;the times and dates&gt; &lt;string&gt;.&lt;tag&gt;&lt;urg&gt;&lt;imp&gt;</t>
+  </si>
+  <si>
+    <t>Raw Start</t>
+  </si>
+  <si>
+    <t>Logged Time</t>
+  </si>
+  <si>
+    <t>Raw Task</t>
+  </si>
+  <si>
+    <t>&lt;date&gt;, &lt;time&gt;</t>
+  </si>
+  <si>
+    <t>3 columns:</t>
+  </si>
+  <si>
+    <t>only 2 column:</t>
+  </si>
+  <si>
+    <t>Log Entry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +107,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,13 +233,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -228,37 +263,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,107 +615,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491817D7-4973-284A-899E-214D547C9E70}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="F4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="16" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="19"/>
-    </row>
-    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="4"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="19"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0.35499999999999998</v>
-      </c>
-      <c r="F5" s="13">
-        <v>0.52700000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D6" s="6"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="E9" s="13">
         <v>5.0599999999999999E-2</v>
       </c>
-      <c r="F8" s="14">
-        <f>1-F5-E5-E8</f>
-        <v>6.7399999999999988E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D9" s="8"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="9"/>
-      <c r="E10" s="12"/>
+      <c r="F9" s="15" t="e">
+        <f>1-#REF!-#REF!-E9</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" s="11"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="12"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Enhance time parsing, session security, and error handling
- Improve time parsing logic with 12-hour inference, explicit datetime handling, and token-based enhancements.
- Add user session validation via User-Agent hash for improved security.
- Enhance error handling for missing or insecure `SECRET_KEY` in production environments.
- Refine date and time input styles for better UI consistency.
- Update tests to ensure time parsing improvements work as intended.
</commit_message>
<xml_diff>
--- a/data given to time tracker.xlsx
+++ b/data given to time tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harsh24/Desktop/Time_Tracker_Pro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B516A533-6465-E344-A874-23024F50D4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6865889-5B59-7F44-8D6A-ACF060190B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16920" xr2:uid="{EB65E887-148F-0A42-8DF7-046F7B9F5706}"/>
   </bookViews>
@@ -239,6 +239,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -275,7 +276,6 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,7 +618,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,10 +663,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -676,27 +676,27 @@
       </c>
       <c r="B5" s="2"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="15"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -706,31 +706,31 @@
         <v>7</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="16"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="14">
         <v>5.0599999999999999E-2</v>
       </c>
-      <c r="F9" s="15" t="e">
+      <c r="F9" s="16" t="e">
         <f>1-#REF!-#REF!-E9</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D10" s="11"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="15"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="12"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="16"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>